<commit_message>
updated for arxiv paper
</commit_message>
<xml_diff>
--- a/RA_Spectra.xlsx
+++ b/RA_Spectra.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30746345-2F7C-4349-BB3A-C147AF136D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2780" windowWidth="38400" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="2780" windowWidth="38400" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="SpectralPlots" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -91,6 +91,12 @@
   <si>
     <t>example 3peak simpleCVNNLS lambda 2</t>
   </si>
+  <si>
+    <t>example 2peak simpleCVNNLS lambda 0.1</t>
+  </si>
+  <si>
+    <t>example 3peak simpleCVNNLS lambda 0.1</t>
+  </si>
 </sst>
 </file>
 
@@ -118,7 +124,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,13 +132,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,83 +475,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3844B0-E6A7-2347-B8AB-DDFFDAAF3289}">
-  <dimension ref="A1:KX9"/>
+  <dimension ref="A1:KX11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="22" width="15.6640625" customWidth="1"/>
-    <col min="23" max="24" width="16.6640625" customWidth="1"/>
-    <col min="25" max="25" width="15.6640625" customWidth="1"/>
-    <col min="26" max="35" width="16.6640625" customWidth="1"/>
-    <col min="36" max="40" width="2.6640625" customWidth="1"/>
-    <col min="41" max="42" width="16.6640625" customWidth="1"/>
-    <col min="43" max="43" width="15.6640625" customWidth="1"/>
-    <col min="44" max="44" width="16.6640625" customWidth="1"/>
-    <col min="45" max="49" width="15.6640625" customWidth="1"/>
-    <col min="50" max="50" width="14.6640625" customWidth="1"/>
-    <col min="51" max="64" width="15.6640625" customWidth="1"/>
-    <col min="65" max="68" width="16.6640625" customWidth="1"/>
-    <col min="69" max="81" width="2.6640625" customWidth="1"/>
-    <col min="82" max="84" width="16.6640625" customWidth="1"/>
-    <col min="85" max="85" width="15.6640625" customWidth="1"/>
-    <col min="86" max="86" width="16.6640625" customWidth="1"/>
-    <col min="87" max="87" width="15.6640625" customWidth="1"/>
-    <col min="88" max="92" width="16.6640625" customWidth="1"/>
-    <col min="93" max="93" width="15.6640625" customWidth="1"/>
-    <col min="94" max="110" width="16.6640625" customWidth="1"/>
-    <col min="111" max="114" width="15.6640625" customWidth="1"/>
-    <col min="115" max="128" width="14.6640625" customWidth="1"/>
-    <col min="129" max="129" width="13.6640625" customWidth="1"/>
-    <col min="130" max="130" width="14.6640625" customWidth="1"/>
-    <col min="131" max="131" width="15.6640625" customWidth="1"/>
-    <col min="132" max="132" width="13.6640625" customWidth="1"/>
-    <col min="133" max="136" width="15.6640625" customWidth="1"/>
-    <col min="137" max="138" width="16.6640625" customWidth="1"/>
-    <col min="139" max="140" width="2.6640625" customWidth="1"/>
-    <col min="141" max="141" width="15.6640625" customWidth="1"/>
-    <col min="142" max="148" width="16.6640625" customWidth="1"/>
-    <col min="149" max="149" width="15.6640625" customWidth="1"/>
-    <col min="150" max="150" width="14.6640625" customWidth="1"/>
-    <col min="151" max="154" width="15.6640625" customWidth="1"/>
-    <col min="155" max="159" width="16.6640625" customWidth="1"/>
-    <col min="160" max="163" width="15.6640625" customWidth="1"/>
-    <col min="164" max="166" width="16.6640625" customWidth="1"/>
-    <col min="167" max="172" width="15.6640625" customWidth="1"/>
-    <col min="173" max="179" width="14.6640625" customWidth="1"/>
-    <col min="180" max="183" width="16.6640625" customWidth="1"/>
-    <col min="184" max="188" width="15.6640625" customWidth="1"/>
-    <col min="189" max="190" width="16.6640625" customWidth="1"/>
-    <col min="191" max="197" width="15.6640625" customWidth="1"/>
-    <col min="198" max="198" width="14.6640625" customWidth="1"/>
-    <col min="199" max="206" width="15.6640625" customWidth="1"/>
-    <col min="207" max="210" width="16.6640625" customWidth="1"/>
-    <col min="211" max="212" width="15.6640625" customWidth="1"/>
-    <col min="213" max="218" width="16.6640625" customWidth="1"/>
-    <col min="219" max="219" width="15.6640625" customWidth="1"/>
-    <col min="220" max="227" width="16.6640625" customWidth="1"/>
-    <col min="228" max="232" width="15.6640625" customWidth="1"/>
-    <col min="233" max="237" width="16.6640625" customWidth="1"/>
-    <col min="238" max="238" width="15.6640625" customWidth="1"/>
-    <col min="239" max="253" width="16.6640625" customWidth="1"/>
-    <col min="254" max="293" width="15.6640625" customWidth="1"/>
-    <col min="294" max="304" width="16.6640625" customWidth="1"/>
-    <col min="305" max="305" width="15.6640625" customWidth="1"/>
-    <col min="306" max="310" width="16.6640625" customWidth="1"/>
-    <col min="311" max="311" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="true"/>
+    <col min="2" max="2" width="15.7109375" customWidth="true"/>
+    <col min="3" max="3" width="13.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="13.7109375" customWidth="true"/>
+    <col min="11" max="11" width="16.7109375" customWidth="true"/>
+    <col min="13" max="13" width="15.7109375" customWidth="true"/>
+    <col min="23" max="23" width="16.7109375" customWidth="true"/>
+    <col min="25" max="25" width="15.7109375" customWidth="true"/>
+    <col min="26" max="26" width="16.7109375" customWidth="true"/>
+    <col min="36" max="36" width="2.7109375" customWidth="true"/>
+    <col min="41" max="41" width="16.7109375" customWidth="true"/>
+    <col min="43" max="43" width="15.7109375" customWidth="true"/>
+    <col min="44" max="44" width="16.7109375" customWidth="true"/>
+    <col min="45" max="45" width="15.7109375" customWidth="true"/>
+    <col min="50" max="50" width="14.7109375" customWidth="true"/>
+    <col min="51" max="51" width="15.7109375" customWidth="true"/>
+    <col min="65" max="65" width="16.7109375" customWidth="true"/>
+    <col min="69" max="69" width="2.7109375" customWidth="true"/>
+    <col min="82" max="82" width="16.7109375" customWidth="true"/>
+    <col min="85" max="85" width="15.7109375" customWidth="true"/>
+    <col min="86" max="86" width="16.7109375" customWidth="true"/>
+    <col min="87" max="87" width="15.7109375" customWidth="true"/>
+    <col min="88" max="88" width="16.7109375" customWidth="true"/>
+    <col min="93" max="93" width="15.7109375" customWidth="true"/>
+    <col min="94" max="94" width="16.7109375" customWidth="true"/>
+    <col min="111" max="111" width="15.7109375" customWidth="true"/>
+    <col min="115" max="115" width="14.7109375" customWidth="true"/>
+    <col min="129" max="129" width="13.7109375" customWidth="true"/>
+    <col min="130" max="130" width="14.7109375" customWidth="true"/>
+    <col min="131" max="131" width="15.7109375" customWidth="true"/>
+    <col min="132" max="132" width="13.7109375" customWidth="true"/>
+    <col min="133" max="133" width="15.7109375" customWidth="true"/>
+    <col min="137" max="137" width="16.7109375" customWidth="true"/>
+    <col min="139" max="139" width="2.7109375" customWidth="true"/>
+    <col min="141" max="141" width="15.7109375" customWidth="true"/>
+    <col min="142" max="142" width="16.7109375" customWidth="true"/>
+    <col min="149" max="149" width="15.7109375" customWidth="true"/>
+    <col min="150" max="150" width="14.7109375" customWidth="true"/>
+    <col min="151" max="151" width="15.7109375" customWidth="true"/>
+    <col min="155" max="155" width="16.7109375" customWidth="true"/>
+    <col min="160" max="160" width="15.7109375" customWidth="true"/>
+    <col min="164" max="164" width="16.7109375" customWidth="true"/>
+    <col min="167" max="167" width="15.7109375" customWidth="true"/>
+    <col min="173" max="173" width="14.7109375" customWidth="true"/>
+    <col min="180" max="180" width="16.7109375" customWidth="true"/>
+    <col min="184" max="184" width="15.7109375" customWidth="true"/>
+    <col min="189" max="189" width="16.7109375" customWidth="true"/>
+    <col min="191" max="191" width="15.7109375" customWidth="true"/>
+    <col min="198" max="198" width="14.7109375" customWidth="true"/>
+    <col min="199" max="199" width="16.7109375" customWidth="true"/>
+    <col min="207" max="207" width="16.7109375" customWidth="true"/>
+    <col min="211" max="211" width="15.7109375" customWidth="true"/>
+    <col min="213" max="213" width="16.7109375" customWidth="true"/>
+    <col min="219" max="219" width="15.7109375" customWidth="true"/>
+    <col min="220" max="220" width="16.7109375" customWidth="true"/>
+    <col min="228" max="228" width="15.7109375" customWidth="true"/>
+    <col min="233" max="233" width="16.7109375" customWidth="true"/>
+    <col min="238" max="238" width="15.7109375" customWidth="true"/>
+    <col min="239" max="239" width="16.7109375" customWidth="true"/>
+    <col min="254" max="254" width="15.7109375" customWidth="true"/>
+    <col min="294" max="294" width="16.7109375" customWidth="true"/>
+    <col min="305" max="305" width="15.7109375" customWidth="true"/>
+    <col min="306" max="306" width="16.7109375" customWidth="true"/>
+    <col min="311" max="311" width="2.6640625" customWidth="true"/>
+    <col min="4" max="4" width="13.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="9" max="9" width="13.7109375" customWidth="true"/>
+    <col min="10" max="10" width="13.7109375" customWidth="true"/>
+    <col min="12" max="12" width="16.7109375" customWidth="true"/>
+    <col min="14" max="14" width="15.7109375" customWidth="true"/>
+    <col min="15" max="15" width="15.7109375" customWidth="true"/>
+    <col min="16" max="16" width="15.7109375" customWidth="true"/>
+    <col min="17" max="17" width="15.7109375" customWidth="true"/>
+    <col min="18" max="18" width="15.7109375" customWidth="true"/>
+    <col min="19" max="19" width="15.7109375" customWidth="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true"/>
+    <col min="21" max="21" width="15.7109375" customWidth="true"/>
+    <col min="22" max="22" width="15.7109375" customWidth="true"/>
+    <col min="24" max="24" width="16.7109375" customWidth="true"/>
+    <col min="27" max="27" width="16.7109375" customWidth="true"/>
+    <col min="28" max="28" width="16.7109375" customWidth="true"/>
+    <col min="29" max="29" width="16.7109375" customWidth="true"/>
+    <col min="30" max="30" width="16.7109375" customWidth="true"/>
+    <col min="31" max="31" width="16.7109375" customWidth="true"/>
+    <col min="32" max="32" width="16.7109375" customWidth="true"/>
+    <col min="33" max="33" width="16.7109375" customWidth="true"/>
+    <col min="34" max="34" width="16.7109375" customWidth="true"/>
+    <col min="35" max="35" width="16.7109375" customWidth="true"/>
+    <col min="37" max="37" width="2.7109375" customWidth="true"/>
+    <col min="38" max="38" width="2.7109375" customWidth="true"/>
+    <col min="39" max="39" width="2.7109375" customWidth="true"/>
+    <col min="40" max="40" width="2.7109375" customWidth="true"/>
+    <col min="42" max="42" width="16.7109375" customWidth="true"/>
+    <col min="46" max="46" width="15.7109375" customWidth="true"/>
+    <col min="47" max="47" width="15.7109375" customWidth="true"/>
+    <col min="48" max="48" width="15.7109375" customWidth="true"/>
+    <col min="49" max="49" width="15.7109375" customWidth="true"/>
+    <col min="52" max="52" width="15.7109375" customWidth="true"/>
+    <col min="53" max="53" width="15.7109375" customWidth="true"/>
+    <col min="54" max="54" width="15.7109375" customWidth="true"/>
+    <col min="55" max="55" width="15.7109375" customWidth="true"/>
+    <col min="56" max="56" width="15.7109375" customWidth="true"/>
+    <col min="57" max="57" width="15.7109375" customWidth="true"/>
+    <col min="58" max="58" width="15.7109375" customWidth="true"/>
+    <col min="59" max="59" width="15.7109375" customWidth="true"/>
+    <col min="60" max="60" width="15.7109375" customWidth="true"/>
+    <col min="61" max="61" width="15.7109375" customWidth="true"/>
+    <col min="62" max="62" width="15.7109375" customWidth="true"/>
+    <col min="63" max="63" width="15.7109375" customWidth="true"/>
+    <col min="64" max="64" width="15.7109375" customWidth="true"/>
+    <col min="66" max="66" width="16.7109375" customWidth="true"/>
+    <col min="67" max="67" width="16.7109375" customWidth="true"/>
+    <col min="68" max="68" width="16.7109375" customWidth="true"/>
+    <col min="70" max="70" width="2.7109375" customWidth="true"/>
+    <col min="71" max="71" width="2.7109375" customWidth="true"/>
+    <col min="72" max="72" width="2.7109375" customWidth="true"/>
+    <col min="73" max="73" width="2.7109375" customWidth="true"/>
+    <col min="74" max="74" width="2.7109375" customWidth="true"/>
+    <col min="75" max="75" width="2.7109375" customWidth="true"/>
+    <col min="76" max="76" width="2.7109375" customWidth="true"/>
+    <col min="77" max="77" width="2.7109375" customWidth="true"/>
+    <col min="78" max="78" width="2.7109375" customWidth="true"/>
+    <col min="79" max="79" width="2.7109375" customWidth="true"/>
+    <col min="80" max="80" width="2.7109375" customWidth="true"/>
+    <col min="81" max="81" width="2.7109375" customWidth="true"/>
+    <col min="83" max="83" width="16.7109375" customWidth="true"/>
+    <col min="84" max="84" width="16.7109375" customWidth="true"/>
+    <col min="89" max="89" width="16.7109375" customWidth="true"/>
+    <col min="90" max="90" width="16.7109375" customWidth="true"/>
+    <col min="91" max="91" width="16.7109375" customWidth="true"/>
+    <col min="92" max="92" width="16.7109375" customWidth="true"/>
+    <col min="95" max="95" width="16.7109375" customWidth="true"/>
+    <col min="96" max="96" width="16.7109375" customWidth="true"/>
+    <col min="97" max="97" width="16.7109375" customWidth="true"/>
+    <col min="98" max="98" width="16.7109375" customWidth="true"/>
+    <col min="99" max="99" width="16.7109375" customWidth="true"/>
+    <col min="100" max="100" width="16.7109375" customWidth="true"/>
+    <col min="101" max="101" width="16.7109375" customWidth="true"/>
+    <col min="102" max="102" width="16.7109375" customWidth="true"/>
+    <col min="103" max="103" width="16.7109375" customWidth="true"/>
+    <col min="104" max="104" width="16.7109375" customWidth="true"/>
+    <col min="105" max="105" width="16.7109375" customWidth="true"/>
+    <col min="106" max="106" width="16.7109375" customWidth="true"/>
+    <col min="107" max="107" width="16.7109375" customWidth="true"/>
+    <col min="108" max="108" width="16.7109375" customWidth="true"/>
+    <col min="109" max="109" width="16.7109375" customWidth="true"/>
+    <col min="110" max="110" width="16.7109375" customWidth="true"/>
+    <col min="112" max="112" width="15.7109375" customWidth="true"/>
+    <col min="113" max="113" width="15.7109375" customWidth="true"/>
+    <col min="114" max="114" width="15.7109375" customWidth="true"/>
+    <col min="116" max="116" width="14.7109375" customWidth="true"/>
+    <col min="117" max="117" width="14.7109375" customWidth="true"/>
+    <col min="118" max="118" width="14.7109375" customWidth="true"/>
+    <col min="119" max="119" width="14.7109375" customWidth="true"/>
+    <col min="120" max="120" width="14.7109375" customWidth="true"/>
+    <col min="121" max="121" width="14.7109375" customWidth="true"/>
+    <col min="122" max="122" width="14.7109375" customWidth="true"/>
+    <col min="123" max="123" width="14.7109375" customWidth="true"/>
+    <col min="124" max="124" width="14.7109375" customWidth="true"/>
+    <col min="125" max="125" width="14.7109375" customWidth="true"/>
+    <col min="126" max="126" width="14.7109375" customWidth="true"/>
+    <col min="127" max="127" width="14.7109375" customWidth="true"/>
+    <col min="128" max="128" width="14.7109375" customWidth="true"/>
+    <col min="134" max="134" width="15.7109375" customWidth="true"/>
+    <col min="135" max="135" width="15.7109375" customWidth="true"/>
+    <col min="136" max="136" width="15.7109375" customWidth="true"/>
+    <col min="138" max="138" width="16.7109375" customWidth="true"/>
+    <col min="140" max="140" width="2.7109375" customWidth="true"/>
+    <col min="143" max="143" width="16.7109375" customWidth="true"/>
+    <col min="144" max="144" width="16.7109375" customWidth="true"/>
+    <col min="145" max="145" width="16.7109375" customWidth="true"/>
+    <col min="146" max="146" width="16.7109375" customWidth="true"/>
+    <col min="147" max="147" width="16.7109375" customWidth="true"/>
+    <col min="148" max="148" width="16.7109375" customWidth="true"/>
+    <col min="152" max="152" width="15.7109375" customWidth="true"/>
+    <col min="153" max="153" width="15.7109375" customWidth="true"/>
+    <col min="154" max="154" width="15.7109375" customWidth="true"/>
+    <col min="156" max="156" width="16.7109375" customWidth="true"/>
+    <col min="157" max="157" width="16.7109375" customWidth="true"/>
+    <col min="158" max="158" width="16.7109375" customWidth="true"/>
+    <col min="159" max="159" width="16.7109375" customWidth="true"/>
+    <col min="161" max="161" width="15.7109375" customWidth="true"/>
+    <col min="162" max="162" width="15.7109375" customWidth="true"/>
+    <col min="163" max="163" width="15.7109375" customWidth="true"/>
+    <col min="165" max="165" width="16.7109375" customWidth="true"/>
+    <col min="166" max="166" width="16.7109375" customWidth="true"/>
+    <col min="168" max="168" width="15.7109375" customWidth="true"/>
+    <col min="169" max="169" width="15.7109375" customWidth="true"/>
+    <col min="170" max="170" width="15.7109375" customWidth="true"/>
+    <col min="171" max="171" width="15.7109375" customWidth="true"/>
+    <col min="172" max="172" width="15.7109375" customWidth="true"/>
+    <col min="174" max="174" width="14.7109375" customWidth="true"/>
+    <col min="175" max="175" width="14.7109375" customWidth="true"/>
+    <col min="176" max="176" width="15.7109375" customWidth="true"/>
+    <col min="177" max="177" width="15.7109375" customWidth="true"/>
+    <col min="178" max="178" width="14.7109375" customWidth="true"/>
+    <col min="179" max="179" width="14.7109375" customWidth="true"/>
+    <col min="181" max="181" width="16.7109375" customWidth="true"/>
+    <col min="182" max="182" width="16.7109375" customWidth="true"/>
+    <col min="183" max="183" width="16.7109375" customWidth="true"/>
+    <col min="185" max="185" width="15.7109375" customWidth="true"/>
+    <col min="186" max="186" width="15.7109375" customWidth="true"/>
+    <col min="187" max="187" width="15.7109375" customWidth="true"/>
+    <col min="188" max="188" width="15.7109375" customWidth="true"/>
+    <col min="190" max="190" width="16.7109375" customWidth="true"/>
+    <col min="192" max="192" width="15.7109375" customWidth="true"/>
+    <col min="193" max="193" width="15.7109375" customWidth="true"/>
+    <col min="194" max="194" width="15.7109375" customWidth="true"/>
+    <col min="195" max="195" width="15.7109375" customWidth="true"/>
+    <col min="196" max="196" width="15.7109375" customWidth="true"/>
+    <col min="197" max="197" width="15.7109375" customWidth="true"/>
+    <col min="200" max="200" width="15.7109375" customWidth="true"/>
+    <col min="201" max="201" width="15.7109375" customWidth="true"/>
+    <col min="202" max="202" width="15.7109375" customWidth="true"/>
+    <col min="203" max="203" width="15.7109375" customWidth="true"/>
+    <col min="204" max="204" width="15.7109375" customWidth="true"/>
+    <col min="205" max="205" width="15.7109375" customWidth="true"/>
+    <col min="206" max="206" width="15.7109375" customWidth="true"/>
+    <col min="208" max="208" width="16.7109375" customWidth="true"/>
+    <col min="209" max="209" width="16.7109375" customWidth="true"/>
+    <col min="210" max="210" width="16.7109375" customWidth="true"/>
+    <col min="212" max="212" width="15.7109375" customWidth="true"/>
+    <col min="214" max="214" width="16.7109375" customWidth="true"/>
+    <col min="215" max="215" width="16.7109375" customWidth="true"/>
+    <col min="216" max="216" width="16.7109375" customWidth="true"/>
+    <col min="217" max="217" width="16.7109375" customWidth="true"/>
+    <col min="218" max="218" width="16.7109375" customWidth="true"/>
+    <col min="221" max="221" width="16.7109375" customWidth="true"/>
+    <col min="222" max="222" width="16.7109375" customWidth="true"/>
+    <col min="223" max="223" width="16.7109375" customWidth="true"/>
+    <col min="224" max="224" width="16.7109375" customWidth="true"/>
+    <col min="225" max="225" width="16.7109375" customWidth="true"/>
+    <col min="226" max="226" width="16.7109375" customWidth="true"/>
+    <col min="227" max="227" width="16.7109375" customWidth="true"/>
+    <col min="229" max="229" width="15.7109375" customWidth="true"/>
+    <col min="230" max="230" width="15.7109375" customWidth="true"/>
+    <col min="231" max="231" width="15.7109375" customWidth="true"/>
+    <col min="232" max="232" width="15.7109375" customWidth="true"/>
+    <col min="234" max="234" width="16.7109375" customWidth="true"/>
+    <col min="235" max="235" width="16.7109375" customWidth="true"/>
+    <col min="236" max="236" width="16.7109375" customWidth="true"/>
+    <col min="237" max="237" width="16.7109375" customWidth="true"/>
+    <col min="240" max="240" width="16.7109375" customWidth="true"/>
+    <col min="241" max="241" width="16.7109375" customWidth="true"/>
+    <col min="242" max="242" width="16.7109375" customWidth="true"/>
+    <col min="243" max="243" width="16.7109375" customWidth="true"/>
+    <col min="244" max="244" width="16.7109375" customWidth="true"/>
+    <col min="245" max="245" width="16.7109375" customWidth="true"/>
+    <col min="246" max="246" width="16.7109375" customWidth="true"/>
+    <col min="247" max="247" width="16.7109375" customWidth="true"/>
+    <col min="248" max="248" width="16.7109375" customWidth="true"/>
+    <col min="249" max="249" width="16.7109375" customWidth="true"/>
+    <col min="250" max="250" width="16.7109375" customWidth="true"/>
+    <col min="251" max="251" width="16.7109375" customWidth="true"/>
+    <col min="252" max="252" width="16.7109375" customWidth="true"/>
+    <col min="253" max="253" width="16.7109375" customWidth="true"/>
+    <col min="255" max="255" width="15.7109375" customWidth="true"/>
+    <col min="256" max="256" width="15.7109375" customWidth="true"/>
+    <col min="257" max="257" width="15.7109375" customWidth="true"/>
+    <col min="258" max="258" width="16.7109375" customWidth="true"/>
+    <col min="259" max="259" width="16.7109375" customWidth="true"/>
+    <col min="260" max="260" width="15.7109375" customWidth="true"/>
+    <col min="261" max="261" width="15.7109375" customWidth="true"/>
+    <col min="262" max="262" width="15.7109375" customWidth="true"/>
+    <col min="263" max="263" width="15.7109375" customWidth="true"/>
+    <col min="264" max="264" width="15.7109375" customWidth="true"/>
+    <col min="265" max="265" width="15.7109375" customWidth="true"/>
+    <col min="266" max="266" width="15.7109375" customWidth="true"/>
+    <col min="267" max="267" width="15.7109375" customWidth="true"/>
+    <col min="268" max="268" width="15.7109375" customWidth="true"/>
+    <col min="269" max="269" width="15.7109375" customWidth="true"/>
+    <col min="270" max="270" width="15.7109375" customWidth="true"/>
+    <col min="271" max="271" width="15.7109375" customWidth="true"/>
+    <col min="272" max="272" width="15.7109375" customWidth="true"/>
+    <col min="273" max="273" width="15.7109375" customWidth="true"/>
+    <col min="274" max="274" width="15.7109375" customWidth="true"/>
+    <col min="275" max="275" width="15.7109375" customWidth="true"/>
+    <col min="276" max="276" width="15.7109375" customWidth="true"/>
+    <col min="277" max="277" width="15.7109375" customWidth="true"/>
+    <col min="278" max="278" width="15.7109375" customWidth="true"/>
+    <col min="279" max="279" width="16.7109375" customWidth="true"/>
+    <col min="280" max="280" width="15.7109375" customWidth="true"/>
+    <col min="281" max="281" width="15.7109375" customWidth="true"/>
+    <col min="282" max="282" width="15.7109375" customWidth="true"/>
+    <col min="283" max="283" width="15.7109375" customWidth="true"/>
+    <col min="284" max="284" width="15.7109375" customWidth="true"/>
+    <col min="285" max="285" width="15.7109375" customWidth="true"/>
+    <col min="286" max="286" width="15.7109375" customWidth="true"/>
+    <col min="287" max="287" width="15.7109375" customWidth="true"/>
+    <col min="288" max="288" width="15.7109375" customWidth="true"/>
+    <col min="289" max="289" width="15.7109375" customWidth="true"/>
+    <col min="290" max="290" width="15.7109375" customWidth="true"/>
+    <col min="291" max="291" width="15.7109375" customWidth="true"/>
+    <col min="292" max="292" width="15.7109375" customWidth="true"/>
+    <col min="293" max="293" width="15.7109375" customWidth="true"/>
+    <col min="295" max="295" width="16.7109375" customWidth="true"/>
+    <col min="296" max="296" width="16.7109375" customWidth="true"/>
+    <col min="297" max="297" width="16.7109375" customWidth="true"/>
+    <col min="298" max="298" width="16.7109375" customWidth="true"/>
+    <col min="299" max="299" width="16.7109375" customWidth="true"/>
+    <col min="300" max="300" width="16.7109375" customWidth="true"/>
+    <col min="301" max="301" width="16.7109375" customWidth="true"/>
+    <col min="302" max="302" width="16.7109375" customWidth="true"/>
+    <col min="303" max="303" width="16.7109375" customWidth="true"/>
+    <col min="304" max="304" width="16.7109375" customWidth="true"/>
+    <col min="307" max="307" width="16.7109375" customWidth="true"/>
+    <col min="308" max="308" width="16.7109375" customWidth="true"/>
+    <col min="309" max="309" width="16.7109375" customWidth="true"/>
+    <col min="310" max="310" width="16.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1507,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2439,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3371,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4303,7 +4556,7 @@
         <v>2.6392963074465387E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -5235,7 +5488,7 @@
         <v>3.3858164103940365E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -6167,7 +6420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -7099,7 +7352,7 @@
         <v>2.6393190252737761E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:310" x14ac:dyDescent="0.2">
+    <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -8028,6 +8281,1870 @@
         <v>0</v>
       </c>
       <c r="KX9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0">
+        <v>0.12675810545779323</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.86112159764413421</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.012120296898072484</v>
+      </c>
+      <c r="F10" s="0">
+        <v>195.17763388595836</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0">
+        <v>3.7479852837183216</v>
+      </c>
+      <c r="I10" s="0">
+        <v>0.46461231766229572</v>
+      </c>
+      <c r="J10" s="0">
+        <v>0.98939023844903295</v>
+      </c>
+      <c r="K10" s="0">
+        <v>0.03448843240441702</v>
+      </c>
+      <c r="L10" s="0">
+        <v>0.045337098144543522</v>
+      </c>
+      <c r="M10" s="0">
+        <v>0.03347618180549617</v>
+      </c>
+      <c r="N10" s="0">
+        <v>0.013078157938102282</v>
+      </c>
+      <c r="O10" s="0">
+        <v>0</v>
+      </c>
+      <c r="P10" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>0</v>
+      </c>
+      <c r="R10" s="0">
+        <v>0</v>
+      </c>
+      <c r="S10" s="0">
+        <v>0</v>
+      </c>
+      <c r="T10" s="0">
+        <v>0</v>
+      </c>
+      <c r="U10" s="0">
+        <v>0</v>
+      </c>
+      <c r="V10" s="0">
+        <v>0</v>
+      </c>
+      <c r="W10" s="0">
+        <v>0</v>
+      </c>
+      <c r="X10" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="BZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="CZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="DZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="ED10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="ER10" s="0">
+        <v>0</v>
+      </c>
+      <c r="ES10" s="0">
+        <v>0</v>
+      </c>
+      <c r="ET10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="EZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="FZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="GQ10" s="0">
+        <v>0.00098809230720129011</v>
+      </c>
+      <c r="GR10" s="0">
+        <v>0.0084804312922657724</v>
+      </c>
+      <c r="GS10" s="0">
+        <v>0.023458996296595605</v>
+      </c>
+      <c r="GT10" s="0">
+        <v>0.044004291832995944</v>
+      </c>
+      <c r="GU10" s="0">
+        <v>0.066653260520984109</v>
+      </c>
+      <c r="GV10" s="0">
+        <v>0.087492533996116839</v>
+      </c>
+      <c r="GW10" s="0">
+        <v>0.10299747497853086</v>
+      </c>
+      <c r="GX10" s="0">
+        <v>0.11062774594495868</v>
+      </c>
+      <c r="GY10" s="0">
+        <v>0.10919037711803756</v>
+      </c>
+      <c r="GZ10" s="0">
+        <v>0.098981499658302288</v>
+      </c>
+      <c r="HA10" s="0">
+        <v>0.081718060087228164</v>
+      </c>
+      <c r="HB10" s="0">
+        <v>0.060270940316996098</v>
+      </c>
+      <c r="HC10" s="0">
+        <v>0.0382109755912056</v>
+      </c>
+      <c r="HD10" s="0">
+        <v>0.01917939165740545</v>
+      </c>
+      <c r="HE10" s="0">
+        <v>0.0060941742176133093</v>
+      </c>
+      <c r="HF10" s="0">
+        <v>0.00020383985372543929</v>
+      </c>
+      <c r="HG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="HZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="ID10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="II10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="IZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JU10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JV10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JW10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JX10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JY10" s="0">
+        <v>0</v>
+      </c>
+      <c r="JZ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KA10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KB10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KC10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KD10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KE10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KF10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KG10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KH10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KI10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KJ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KK10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KL10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KM10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KN10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KO10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KP10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KQ10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KR10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KS10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KT10" s="0">
+        <v>0</v>
+      </c>
+      <c r="KU10" s="0">
+        <v>0.0008530400704241175</v>
+      </c>
+      <c r="KV10" s="0">
+        <v>0.0029417316500904736</v>
+      </c>
+      <c r="KW10" s="0">
+        <v>0.0045606345227619379</v>
+      </c>
+      <c r="KX10" s="0">
+        <v>0.0037287247426960996</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="0">
+        <v>0.029172953736922063</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0.67770210024818578</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0.29312494601489225</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0">
+        <v>189.43733384893719</v>
+      </c>
+      <c r="G11" s="0">
+        <v>5.8691587778529772</v>
+      </c>
+      <c r="H11" s="0">
+        <v>1.0503542901456222</v>
+      </c>
+      <c r="I11" s="0">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0">
+        <v>0.99452262749450526</v>
+      </c>
+      <c r="K11" s="0">
+        <v>0.0028549741638439958</v>
+      </c>
+      <c r="L11" s="0">
+        <v>0.0050594188125148458</v>
+      </c>
+      <c r="M11" s="0">
+        <v>0.0061551041686401286</v>
+      </c>
+      <c r="N11" s="0">
+        <v>0.0059900572341421363</v>
+      </c>
+      <c r="O11" s="0">
+        <v>0.0047571845410361979</v>
+      </c>
+      <c r="P11" s="0">
+        <v>0.0029500566689755502</v>
+      </c>
+      <c r="Q11" s="0">
+        <v>0.001228108397313993</v>
+      </c>
+      <c r="R11" s="0">
+        <v>0.0001832886720007142</v>
+      </c>
+      <c r="S11" s="0">
+        <v>0</v>
+      </c>
+      <c r="T11" s="0">
+        <v>0</v>
+      </c>
+      <c r="U11" s="0">
+        <v>0</v>
+      </c>
+      <c r="V11" s="0">
+        <v>0</v>
+      </c>
+      <c r="W11" s="0">
+        <v>0</v>
+      </c>
+      <c r="X11" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="BZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="CZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="DZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="ED11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="ER11" s="0">
+        <v>0</v>
+      </c>
+      <c r="ES11" s="0">
+        <v>0</v>
+      </c>
+      <c r="ET11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="EZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="FT11" s="0">
+        <v>0.0017210641356524079</v>
+      </c>
+      <c r="FU11" s="0">
+        <v>0.0069328483715579052</v>
+      </c>
+      <c r="FV11" s="0">
+        <v>0.015788077486314354</v>
+      </c>
+      <c r="FW11" s="0">
+        <v>0.027394261144711187</v>
+      </c>
+      <c r="FX11" s="0">
+        <v>0.040284045106715426</v>
+      </c>
+      <c r="FY11" s="0">
+        <v>0.052791657506426858</v>
+      </c>
+      <c r="FZ11" s="0">
+        <v>0.063342746188487314</v>
+      </c>
+      <c r="GA11" s="0">
+        <v>0.070664719076811183</v>
+      </c>
+      <c r="GB11" s="0">
+        <v>0.073924497476387102</v>
+      </c>
+      <c r="GC11" s="0">
+        <v>0.072800374061815623</v>
+      </c>
+      <c r="GD11" s="0">
+        <v>0.067494435048119958</v>
+      </c>
+      <c r="GE11" s="0">
+        <v>0.058691761591945502</v>
+      </c>
+      <c r="GF11" s="0">
+        <v>0.047472370712482392</v>
+      </c>
+      <c r="GG11" s="0">
+        <v>0.035181592767183766</v>
+      </c>
+      <c r="GH11" s="0">
+        <v>0.02326431252465307</v>
+      </c>
+      <c r="GI11" s="0">
+        <v>0.013068225830409175</v>
+      </c>
+      <c r="GJ11" s="0">
+        <v>0.0056209853658790061</v>
+      </c>
+      <c r="GK11" s="0">
+        <v>0.0013858285834039436</v>
+      </c>
+      <c r="GL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="GZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="HZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="ID11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="II11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="IX11" s="0">
+        <v>1.6720809932419976e-05</v>
+      </c>
+      <c r="IY11" s="0">
+        <v>0.00065343442506500201</v>
+      </c>
+      <c r="IZ11" s="0">
+        <v>0.0021905958759228842</v>
+      </c>
+      <c r="JA11" s="0">
+        <v>0.0046610667059048903</v>
+      </c>
+      <c r="JB11" s="0">
+        <v>0.0079179981927950879</v>
+      </c>
+      <c r="JC11" s="0">
+        <v>0.011695321976689562</v>
+      </c>
+      <c r="JD11" s="0">
+        <v>0.015660815768491682</v>
+      </c>
+      <c r="JE11" s="0">
+        <v>0.019461730806866199</v>
+      </c>
+      <c r="JF11" s="0">
+        <v>0.022762985710536057</v>
+      </c>
+      <c r="JG11" s="0">
+        <v>0.025277948341309846</v>
+      </c>
+      <c r="JH11" s="0">
+        <v>0.026791843261147127</v>
+      </c>
+      <c r="JI11" s="0">
+        <v>0.02717783734869712</v>
+      </c>
+      <c r="JJ11" s="0">
+        <v>0.026405870148102556</v>
+      </c>
+      <c r="JK11" s="0">
+        <v>0.024544308579049059</v>
+      </c>
+      <c r="JL11" s="0">
+        <v>0.02175451776043218</v>
+      </c>
+      <c r="JM11" s="0">
+        <v>0.018278450912763835</v>
+      </c>
+      <c r="JN11" s="0">
+        <v>0.014419371632239074</v>
+      </c>
+      <c r="JO11" s="0">
+        <v>0.010515831298410017</v>
+      </c>
+      <c r="JP11" s="0">
+        <v>0.0069090330136741896</v>
+      </c>
+      <c r="JQ11" s="0">
+        <v>0.0039037213061689237</v>
+      </c>
+      <c r="JR11" s="0">
+        <v>0.0017227438861989754</v>
+      </c>
+      <c r="JS11" s="0">
+        <v>0.00045543805946873073</v>
+      </c>
+      <c r="JT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="JU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="JV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="JW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="JX11" s="0">
+        <v>0</v>
+      </c>
+      <c r="JY11" s="0">
+        <v>0</v>
+      </c>
+      <c r="JZ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KA11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KB11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KC11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KD11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KE11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KF11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KG11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KH11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KI11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KJ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KK11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KL11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KM11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KN11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KO11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KP11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KQ11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KR11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KS11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KT11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KU11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KV11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KW11" s="0">
+        <v>0</v>
+      </c>
+      <c r="KX11" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>